<commit_message>
Atualiza excel - Access Control
</commit_message>
<xml_diff>
--- a/v4-ASVS-checklist-en.xlsx
+++ b/v4-ASVS-checklist-en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leandro\Desktop\Faculdade\2º Ano\DESOFS\desofs2024_M1C_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CE2E51-8B70-415D-B767-E43E7251D6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF43845B-0B13-4C3F-9E79-DC5F28181FFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASVS Results" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="694">
   <si>
     <t>Security Category</t>
   </si>
@@ -3255,6 +3255,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3264,7 +3265,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3533,7 +3533,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>88.888888888888886</c:v>
@@ -3566,7 +3566,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27.450980392156865</c:v>
+                  <c:v>30.980392156862745</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4172,7 +4172,7 @@
       </c>
       <c r="B5" s="9">
         <f>COUNTIF('Access Control'!G2:G11,"Valid")</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C5" s="10">
         <f>COUNTIF('Access Control'!G2:G11,"&lt;&gt;Not Applicable")</f>
@@ -4180,7 +4180,7 @@
       </c>
       <c r="D5" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E5" s="12"/>
     </row>
@@ -4371,7 +4371,7 @@
       </c>
       <c r="B16" s="9">
         <f>SUM(B2:B15)</f>
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C16" s="10">
         <f>SUM(C2:C15)</f>
@@ -4379,7 +4379,7 @@
       </c>
       <c r="D16" s="11">
         <f t="shared" si="0"/>
-        <v>27.450980392156865</v>
+        <v>30.980392156862745</v>
       </c>
       <c r="E16" s="12"/>
     </row>
@@ -4448,7 +4448,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="48" customHeight="1">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="123" t="s">
         <v>505</v>
       </c>
       <c r="B2" s="63" t="s">
@@ -4472,7 +4472,7 @@
       <c r="J2" s="66"/>
     </row>
     <row r="3" spans="1:10" ht="31.2">
-      <c r="A3" s="122"/>
+      <c r="A3" s="123"/>
       <c r="B3" s="63" t="s">
         <v>508</v>
       </c>
@@ -4494,7 +4494,7 @@
       <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:10" ht="31.2">
-      <c r="A4" s="122"/>
+      <c r="A4" s="123"/>
       <c r="B4" s="63" t="s">
         <v>510</v>
       </c>
@@ -4516,7 +4516,7 @@
       <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="63.75" customHeight="1">
-      <c r="A5" s="122" t="s">
+      <c r="A5" s="123" t="s">
         <v>512</v>
       </c>
       <c r="B5" s="63" t="s">
@@ -4540,7 +4540,7 @@
       <c r="J5" s="33"/>
     </row>
     <row r="6" spans="1:10" ht="62.4">
-      <c r="A6" s="122"/>
+      <c r="A6" s="123"/>
       <c r="B6" s="63" t="s">
         <v>515</v>
       </c>
@@ -4562,7 +4562,7 @@
       <c r="J6" s="33"/>
     </row>
     <row r="7" spans="1:10" ht="31.2">
-      <c r="A7" s="122"/>
+      <c r="A7" s="123"/>
       <c r="B7" s="63" t="s">
         <v>517</v>
       </c>
@@ -4584,7 +4584,7 @@
       <c r="J7" s="33"/>
     </row>
     <row r="8" spans="1:10" ht="31.2">
-      <c r="A8" s="122"/>
+      <c r="A8" s="123"/>
       <c r="B8" s="63" t="s">
         <v>519</v>
       </c>
@@ -4606,7 +4606,7 @@
       <c r="J8" s="33"/>
     </row>
     <row r="9" spans="1:10" ht="15.6">
-      <c r="A9" s="122"/>
+      <c r="A9" s="123"/>
       <c r="B9" s="63" t="s">
         <v>521</v>
       </c>
@@ -4651,7 +4651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -4725,7 +4725,7 @@
       <c r="J2" s="66"/>
     </row>
     <row r="3" spans="1:10" ht="48" customHeight="1">
-      <c r="A3" s="122" t="s">
+      <c r="A3" s="123" t="s">
         <v>526</v>
       </c>
       <c r="B3" s="63" t="s">
@@ -4749,7 +4749,7 @@
       <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:10" ht="31.2">
-      <c r="A4" s="122"/>
+      <c r="A4" s="123"/>
       <c r="B4" s="63" t="s">
         <v>529</v>
       </c>
@@ -4771,7 +4771,7 @@
       <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="78">
-      <c r="A5" s="122"/>
+      <c r="A5" s="123"/>
       <c r="B5" s="63" t="s">
         <v>531</v>
       </c>
@@ -4793,7 +4793,7 @@
       <c r="J5" s="33"/>
     </row>
     <row r="6" spans="1:10" ht="31.2">
-      <c r="A6" s="122"/>
+      <c r="A6" s="123"/>
       <c r="B6" s="63" t="s">
         <v>533</v>
       </c>
@@ -4815,7 +4815,7 @@
       <c r="J6" s="33"/>
     </row>
     <row r="7" spans="1:10" ht="31.2">
-      <c r="A7" s="122"/>
+      <c r="A7" s="123"/>
       <c r="B7" s="63" t="s">
         <v>535</v>
       </c>
@@ -4837,7 +4837,7 @@
       <c r="J7" s="33"/>
     </row>
     <row r="8" spans="1:10" ht="31.2">
-      <c r="A8" s="122"/>
+      <c r="A8" s="123"/>
       <c r="B8" s="63" t="s">
         <v>537</v>
       </c>
@@ -4859,7 +4859,7 @@
       <c r="J8" s="33"/>
     </row>
     <row r="9" spans="1:10" ht="48" customHeight="1">
-      <c r="A9" s="122" t="s">
+      <c r="A9" s="123" t="s">
         <v>539</v>
       </c>
       <c r="B9" s="63" t="s">
@@ -4883,7 +4883,7 @@
       <c r="J9" s="33"/>
     </row>
     <row r="10" spans="1:10" ht="62.4">
-      <c r="A10" s="122"/>
+      <c r="A10" s="123"/>
       <c r="B10" s="63" t="s">
         <v>542</v>
       </c>
@@ -4905,7 +4905,7 @@
       <c r="J10" s="33"/>
     </row>
     <row r="11" spans="1:10" ht="93.6">
-      <c r="A11" s="122"/>
+      <c r="A11" s="123"/>
       <c r="B11" s="63" t="s">
         <v>544</v>
       </c>
@@ -5000,7 +5000,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="123" t="s">
         <v>546</v>
       </c>
       <c r="B2" s="63" t="s">
@@ -5022,7 +5022,7 @@
       <c r="J2" s="66"/>
     </row>
     <row r="3" spans="1:10" ht="46.8">
-      <c r="A3" s="122"/>
+      <c r="A3" s="123"/>
       <c r="B3" s="63" t="s">
         <v>549</v>
       </c>
@@ -5042,7 +5042,7 @@
       <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:10" ht="31.2">
-      <c r="A4" s="122"/>
+      <c r="A4" s="123"/>
       <c r="B4" s="63" t="s">
         <v>551</v>
       </c>
@@ -5062,7 +5062,7 @@
       <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="46.8">
-      <c r="A5" s="122"/>
+      <c r="A5" s="123"/>
       <c r="B5" s="63" t="s">
         <v>553</v>
       </c>
@@ -5082,7 +5082,7 @@
       <c r="J5" s="33"/>
     </row>
     <row r="6" spans="1:10" ht="46.8">
-      <c r="A6" s="122"/>
+      <c r="A6" s="123"/>
       <c r="B6" s="63" t="s">
         <v>555</v>
       </c>
@@ -5102,7 +5102,7 @@
       <c r="J6" s="33"/>
     </row>
     <row r="7" spans="1:10" ht="36" customHeight="1">
-      <c r="A7" s="122"/>
+      <c r="A7" s="123"/>
       <c r="B7" s="63" t="s">
         <v>557</v>
       </c>
@@ -5122,7 +5122,7 @@
       <c r="J7" s="33"/>
     </row>
     <row r="8" spans="1:10" ht="66.75" customHeight="1">
-      <c r="A8" s="122"/>
+      <c r="A8" s="123"/>
       <c r="B8" s="63" t="s">
         <v>559</v>
       </c>
@@ -5142,7 +5142,7 @@
       <c r="J8" s="33"/>
     </row>
     <row r="9" spans="1:10" ht="31.2">
-      <c r="A9" s="122"/>
+      <c r="A9" s="123"/>
       <c r="B9" s="63" t="s">
         <v>561</v>
       </c>
@@ -5234,7 +5234,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="123" t="s">
         <v>563</v>
       </c>
       <c r="B2" s="63" t="s">
@@ -5256,7 +5256,7 @@
       <c r="J2" s="66"/>
     </row>
     <row r="3" spans="1:10" ht="46.8">
-      <c r="A3" s="122"/>
+      <c r="A3" s="123"/>
       <c r="B3" s="63" t="s">
         <v>566</v>
       </c>
@@ -5276,7 +5276,7 @@
       <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:10" ht="46.8">
-      <c r="A4" s="122"/>
+      <c r="A4" s="123"/>
       <c r="B4" s="63" t="s">
         <v>568</v>
       </c>
@@ -5318,7 +5318,7 @@
       <c r="J5" s="33"/>
     </row>
     <row r="6" spans="1:10" ht="48" customHeight="1">
-      <c r="A6" s="122" t="s">
+      <c r="A6" s="123" t="s">
         <v>573</v>
       </c>
       <c r="B6" s="63" t="s">
@@ -5340,7 +5340,7 @@
       <c r="J6" s="33"/>
     </row>
     <row r="7" spans="1:10" ht="31.2">
-      <c r="A7" s="122"/>
+      <c r="A7" s="123"/>
       <c r="B7" s="63" t="s">
         <v>576</v>
       </c>
@@ -5360,7 +5360,7 @@
       <c r="J7" s="33"/>
     </row>
     <row r="8" spans="1:10" ht="46.8">
-      <c r="A8" s="122"/>
+      <c r="A8" s="123"/>
       <c r="B8" s="63" t="s">
         <v>578</v>
       </c>
@@ -5380,7 +5380,7 @@
       <c r="J8" s="33"/>
     </row>
     <row r="9" spans="1:10" ht="62.4">
-      <c r="A9" s="122"/>
+      <c r="A9" s="123"/>
       <c r="B9" s="63" t="s">
         <v>580</v>
       </c>
@@ -5400,7 +5400,7 @@
       <c r="J9" s="33"/>
     </row>
     <row r="10" spans="1:10" ht="31.2">
-      <c r="A10" s="122"/>
+      <c r="A10" s="123"/>
       <c r="B10" s="63" t="s">
         <v>582</v>
       </c>
@@ -5420,7 +5420,7 @@
       <c r="J10" s="33"/>
     </row>
     <row r="11" spans="1:10" ht="46.8">
-      <c r="A11" s="122"/>
+      <c r="A11" s="123"/>
       <c r="B11" s="63" t="s">
         <v>584</v>
       </c>
@@ -5440,7 +5440,7 @@
       <c r="J11" s="33"/>
     </row>
     <row r="12" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A12" s="122" t="s">
+      <c r="A12" s="123" t="s">
         <v>586</v>
       </c>
       <c r="B12" s="63" t="s">
@@ -5462,7 +5462,7 @@
       <c r="J12" s="33"/>
     </row>
     <row r="13" spans="1:10" ht="31.2">
-      <c r="A13" s="122"/>
+      <c r="A13" s="123"/>
       <c r="B13" s="63" t="s">
         <v>589</v>
       </c>
@@ -5482,7 +5482,7 @@
       <c r="J13" s="33"/>
     </row>
     <row r="14" spans="1:10" ht="79.5" customHeight="1">
-      <c r="A14" s="122" t="s">
+      <c r="A14" s="123" t="s">
         <v>591</v>
       </c>
       <c r="B14" s="63" t="s">
@@ -5504,7 +5504,7 @@
       <c r="J14" s="33"/>
     </row>
     <row r="15" spans="1:10" ht="31.2">
-      <c r="A15" s="122"/>
+      <c r="A15" s="123"/>
       <c r="B15" s="63" t="s">
         <v>594</v>
       </c>
@@ -5620,7 +5620,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="48" customHeight="1">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="123" t="s">
         <v>599</v>
       </c>
       <c r="B2" s="63" t="s">
@@ -5642,7 +5642,7 @@
       <c r="J2" s="66"/>
     </row>
     <row r="3" spans="1:10" ht="15.6">
-      <c r="A3" s="122"/>
+      <c r="A3" s="123"/>
       <c r="B3" s="63" t="s">
         <v>602</v>
       </c>
@@ -5664,7 +5664,7 @@
       <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:10" ht="31.2">
-      <c r="A4" s="122"/>
+      <c r="A4" s="123"/>
       <c r="B4" s="63" t="s">
         <v>604</v>
       </c>
@@ -5684,7 +5684,7 @@
       <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="46.8">
-      <c r="A5" s="122"/>
+      <c r="A5" s="123"/>
       <c r="B5" s="63" t="s">
         <v>606</v>
       </c>
@@ -5704,7 +5704,7 @@
       <c r="J5" s="33"/>
     </row>
     <row r="6" spans="1:10" ht="46.8">
-      <c r="A6" s="122"/>
+      <c r="A6" s="123"/>
       <c r="B6" s="63" t="s">
         <v>608</v>
       </c>
@@ -5724,7 +5724,7 @@
       <c r="J6" s="33"/>
     </row>
     <row r="7" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A7" s="122" t="s">
+      <c r="A7" s="123" t="s">
         <v>610</v>
       </c>
       <c r="B7" s="63" t="s">
@@ -5746,7 +5746,7 @@
       <c r="J7" s="33"/>
     </row>
     <row r="8" spans="1:10" ht="15.6">
-      <c r="A8" s="122"/>
+      <c r="A8" s="123"/>
       <c r="B8" s="63" t="s">
         <v>613</v>
       </c>
@@ -5766,7 +5766,7 @@
       <c r="J8" s="33"/>
     </row>
     <row r="9" spans="1:10" ht="46.8">
-      <c r="A9" s="122"/>
+      <c r="A9" s="123"/>
       <c r="B9" s="63" t="s">
         <v>615</v>
       </c>
@@ -5786,7 +5786,7 @@
       <c r="J9" s="33"/>
     </row>
     <row r="10" spans="1:10" ht="15.6">
-      <c r="A10" s="122"/>
+      <c r="A10" s="123"/>
       <c r="B10" s="63" t="s">
         <v>617</v>
       </c>
@@ -5808,7 +5808,7 @@
       <c r="J10" s="33"/>
     </row>
     <row r="11" spans="1:10" ht="31.2">
-      <c r="A11" s="122"/>
+      <c r="A11" s="123"/>
       <c r="B11" s="63" t="s">
         <v>619</v>
       </c>
@@ -5828,7 +5828,7 @@
       <c r="J11" s="33"/>
     </row>
     <row r="12" spans="1:10" ht="93.6">
-      <c r="A12" s="122"/>
+      <c r="A12" s="123"/>
       <c r="B12" s="63" t="s">
         <v>621</v>
       </c>
@@ -5848,7 +5848,7 @@
       <c r="J12" s="33"/>
     </row>
     <row r="13" spans="1:10" ht="48" customHeight="1">
-      <c r="A13" s="122" t="s">
+      <c r="A13" s="123" t="s">
         <v>623</v>
       </c>
       <c r="B13" s="63" t="s">
@@ -5870,7 +5870,7 @@
       <c r="J13" s="33"/>
     </row>
     <row r="14" spans="1:10" ht="31.2">
-      <c r="A14" s="122"/>
+      <c r="A14" s="123"/>
       <c r="B14" s="63" t="s">
         <v>626</v>
       </c>
@@ -5890,7 +5890,7 @@
       <c r="J14" s="33"/>
     </row>
     <row r="15" spans="1:10" ht="63.75" customHeight="1">
-      <c r="A15" s="122" t="s">
+      <c r="A15" s="123" t="s">
         <v>628</v>
       </c>
       <c r="B15" s="63" t="s">
@@ -5912,7 +5912,7 @@
       <c r="J15" s="33"/>
     </row>
     <row r="16" spans="1:10" ht="31.2">
-      <c r="A16" s="122"/>
+      <c r="A16" s="123"/>
       <c r="B16" s="63" t="s">
         <v>631</v>
       </c>
@@ -6007,7 +6007,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="48" customHeight="1">
-      <c r="A2" s="123" t="s">
+      <c r="A2" s="124" t="s">
         <v>633</v>
       </c>
       <c r="B2" s="100" t="s">
@@ -6027,7 +6027,7 @@
       <c r="J2" s="106"/>
     </row>
     <row r="3" spans="1:10" ht="46.8">
-      <c r="A3" s="123"/>
+      <c r="A3" s="124"/>
       <c r="B3" s="63" t="s">
         <v>636</v>
       </c>
@@ -6047,7 +6047,7 @@
       <c r="J3" s="112"/>
     </row>
     <row r="4" spans="1:10" ht="31.2">
-      <c r="A4" s="123"/>
+      <c r="A4" s="124"/>
       <c r="B4" s="63" t="s">
         <v>638</v>
       </c>
@@ -6067,7 +6067,7 @@
       <c r="J4" s="112"/>
     </row>
     <row r="5" spans="1:10" ht="46.8">
-      <c r="A5" s="123"/>
+      <c r="A5" s="124"/>
       <c r="B5" s="63" t="s">
         <v>640</v>
       </c>
@@ -6085,7 +6085,7 @@
       <c r="J5" s="112"/>
     </row>
     <row r="6" spans="1:10" ht="31.2">
-      <c r="A6" s="123"/>
+      <c r="A6" s="124"/>
       <c r="B6" s="63" t="s">
         <v>642</v>
       </c>
@@ -6103,7 +6103,7 @@
       <c r="J6" s="112"/>
     </row>
     <row r="7" spans="1:10" ht="48" customHeight="1">
-      <c r="A7" s="122" t="s">
+      <c r="A7" s="123" t="s">
         <v>644</v>
       </c>
       <c r="B7" s="63" t="s">
@@ -6125,7 +6125,7 @@
       <c r="J7" s="112"/>
     </row>
     <row r="8" spans="1:10" ht="31.2">
-      <c r="A8" s="122"/>
+      <c r="A8" s="123"/>
       <c r="B8" s="63" t="s">
         <v>647</v>
       </c>
@@ -6145,7 +6145,7 @@
       <c r="J8" s="112"/>
     </row>
     <row r="9" spans="1:10" ht="46.8">
-      <c r="A9" s="122"/>
+      <c r="A9" s="123"/>
       <c r="B9" s="63" t="s">
         <v>649</v>
       </c>
@@ -6165,7 +6165,7 @@
       <c r="J9" s="112"/>
     </row>
     <row r="10" spans="1:10" ht="46.8">
-      <c r="A10" s="122"/>
+      <c r="A10" s="123"/>
       <c r="B10" s="63" t="s">
         <v>651</v>
       </c>
@@ -6185,7 +6185,7 @@
       <c r="J10" s="112"/>
     </row>
     <row r="11" spans="1:10" ht="31.2">
-      <c r="A11" s="122"/>
+      <c r="A11" s="123"/>
       <c r="B11" s="63" t="s">
         <v>653</v>
       </c>
@@ -6203,7 +6203,7 @@
       <c r="J11" s="112"/>
     </row>
     <row r="12" spans="1:10" ht="46.8">
-      <c r="A12" s="122"/>
+      <c r="A12" s="123"/>
       <c r="B12" s="63" t="s">
         <v>655</v>
       </c>
@@ -6223,7 +6223,7 @@
       <c r="J12" s="112"/>
     </row>
     <row r="13" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A13" s="122" t="s">
+      <c r="A13" s="123" t="s">
         <v>657</v>
       </c>
       <c r="B13" s="63" t="s">
@@ -6247,7 +6247,7 @@
       <c r="J13" s="112"/>
     </row>
     <row r="14" spans="1:10" ht="46.8">
-      <c r="A14" s="122"/>
+      <c r="A14" s="123"/>
       <c r="B14" s="63" t="s">
         <v>660</v>
       </c>
@@ -6267,7 +6267,7 @@
       <c r="J14" s="112"/>
     </row>
     <row r="15" spans="1:10" ht="31.2">
-      <c r="A15" s="122"/>
+      <c r="A15" s="123"/>
       <c r="B15" s="63" t="s">
         <v>662</v>
       </c>
@@ -6287,7 +6287,7 @@
       <c r="J15" s="112"/>
     </row>
     <row r="16" spans="1:10" ht="48" customHeight="1">
-      <c r="A16" s="122" t="s">
+      <c r="A16" s="123" t="s">
         <v>664</v>
       </c>
       <c r="B16" s="63" t="s">
@@ -6309,7 +6309,7 @@
       <c r="J16" s="112"/>
     </row>
     <row r="17" spans="1:10" ht="31.2">
-      <c r="A17" s="122"/>
+      <c r="A17" s="123"/>
       <c r="B17" s="63" t="s">
         <v>667</v>
       </c>
@@ -6329,7 +6329,7 @@
       <c r="J17" s="112"/>
     </row>
     <row r="18" spans="1:10" ht="31.2">
-      <c r="A18" s="122"/>
+      <c r="A18" s="123"/>
       <c r="B18" s="63" t="s">
         <v>669</v>
       </c>
@@ -6349,7 +6349,7 @@
       <c r="J18" s="112"/>
     </row>
     <row r="19" spans="1:10" ht="15.6">
-      <c r="A19" s="122"/>
+      <c r="A19" s="123"/>
       <c r="B19" s="63" t="s">
         <v>671</v>
       </c>
@@ -6369,7 +6369,7 @@
       <c r="J19" s="112"/>
     </row>
     <row r="20" spans="1:10" ht="31.2">
-      <c r="A20" s="122"/>
+      <c r="A20" s="123"/>
       <c r="B20" s="63" t="s">
         <v>673</v>
       </c>
@@ -6389,7 +6389,7 @@
       <c r="J20" s="112"/>
     </row>
     <row r="21" spans="1:10" ht="31.2">
-      <c r="A21" s="122"/>
+      <c r="A21" s="123"/>
       <c r="B21" s="63" t="s">
         <v>675</v>
       </c>
@@ -6409,7 +6409,7 @@
       <c r="J21" s="112"/>
     </row>
     <row r="22" spans="1:10" ht="62.4">
-      <c r="A22" s="122"/>
+      <c r="A22" s="123"/>
       <c r="B22" s="63" t="s">
         <v>677</v>
       </c>
@@ -6429,7 +6429,7 @@
       <c r="J22" s="112"/>
     </row>
     <row r="23" spans="1:10" ht="48" customHeight="1">
-      <c r="A23" s="122" t="s">
+      <c r="A23" s="123" t="s">
         <v>679</v>
       </c>
       <c r="B23" s="63" t="s">
@@ -6451,7 +6451,7 @@
       <c r="J23" s="112"/>
     </row>
     <row r="24" spans="1:10" ht="31.2">
-      <c r="A24" s="122"/>
+      <c r="A24" s="123"/>
       <c r="B24" s="63" t="s">
         <v>682</v>
       </c>
@@ -6471,7 +6471,7 @@
       <c r="J24" s="112"/>
     </row>
     <row r="25" spans="1:10" ht="46.8">
-      <c r="A25" s="122"/>
+      <c r="A25" s="123"/>
       <c r="B25" s="63" t="s">
         <v>684</v>
       </c>
@@ -6491,7 +6491,7 @@
       <c r="J25" s="112"/>
     </row>
     <row r="26" spans="1:10" ht="31.2">
-      <c r="A26" s="122"/>
+      <c r="A26" s="123"/>
       <c r="B26" s="63" t="s">
         <v>686</v>
       </c>
@@ -6588,7 +6588,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="26" customFormat="1" ht="58.2" customHeight="1">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="122" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -6608,7 +6608,7 @@
       <c r="J2" s="25"/>
     </row>
     <row r="3" spans="1:10" s="26" customFormat="1" ht="62.4">
-      <c r="A3" s="121"/>
+      <c r="A3" s="122"/>
       <c r="B3" s="19" t="s">
         <v>33</v>
       </c>
@@ -6628,7 +6628,7 @@
       <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" s="26" customFormat="1" ht="62.4">
-      <c r="A4" s="121"/>
+      <c r="A4" s="122"/>
       <c r="B4" s="19" t="s">
         <v>35</v>
       </c>
@@ -6648,7 +6648,7 @@
       <c r="J4" s="32"/>
     </row>
     <row r="5" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A5" s="121"/>
+      <c r="A5" s="122"/>
       <c r="B5" s="19" t="s">
         <v>37</v>
       </c>
@@ -6668,7 +6668,7 @@
       <c r="J5" s="32"/>
     </row>
     <row r="6" spans="1:10" s="26" customFormat="1" ht="62.4">
-      <c r="A6" s="121"/>
+      <c r="A6" s="122"/>
       <c r="B6" s="19" t="s">
         <v>39</v>
       </c>
@@ -6688,7 +6688,7 @@
       <c r="J6" s="32"/>
     </row>
     <row r="7" spans="1:10" s="26" customFormat="1" ht="78">
-      <c r="A7" s="121"/>
+      <c r="A7" s="122"/>
       <c r="B7" s="19" t="s">
         <v>41</v>
       </c>
@@ -6708,7 +6708,7 @@
       <c r="J7" s="32"/>
     </row>
     <row r="8" spans="1:10" s="26" customFormat="1" ht="46.8">
-      <c r="A8" s="121"/>
+      <c r="A8" s="122"/>
       <c r="B8" s="19" t="s">
         <v>43</v>
       </c>
@@ -6728,7 +6728,7 @@
       <c r="J8" s="32"/>
     </row>
     <row r="9" spans="1:10" s="26" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A9" s="121" t="s">
+      <c r="A9" s="122" t="s">
         <v>45</v>
       </c>
       <c r="B9" s="19" t="s">
@@ -6750,7 +6750,7 @@
       <c r="J9" s="32"/>
     </row>
     <row r="10" spans="1:10" s="26" customFormat="1" ht="78">
-      <c r="A10" s="121"/>
+      <c r="A10" s="122"/>
       <c r="B10" s="19" t="s">
         <v>48</v>
       </c>
@@ -6770,7 +6770,7 @@
       <c r="J10" s="32"/>
     </row>
     <row r="11" spans="1:10" s="26" customFormat="1" ht="62.4">
-      <c r="A11" s="121"/>
+      <c r="A11" s="122"/>
       <c r="B11" s="19" t="s">
         <v>50</v>
       </c>
@@ -6790,7 +6790,7 @@
       <c r="J11" s="32"/>
     </row>
     <row r="12" spans="1:10" s="26" customFormat="1" ht="62.4">
-      <c r="A12" s="121"/>
+      <c r="A12" s="122"/>
       <c r="B12" s="19" t="s">
         <v>52</v>
       </c>
@@ -6828,7 +6828,7 @@
       <c r="J13" s="32"/>
     </row>
     <row r="14" spans="1:10" s="26" customFormat="1" ht="48" customHeight="1">
-      <c r="A14" s="121" t="s">
+      <c r="A14" s="122" t="s">
         <v>57</v>
       </c>
       <c r="B14" s="19" t="s">
@@ -6850,7 +6850,7 @@
       <c r="J14" s="33"/>
     </row>
     <row r="15" spans="1:10" s="26" customFormat="1" ht="15.6">
-      <c r="A15" s="121"/>
+      <c r="A15" s="122"/>
       <c r="B15" s="19" t="s">
         <v>60</v>
       </c>
@@ -6872,7 +6872,7 @@
       <c r="J15" s="33"/>
     </row>
     <row r="16" spans="1:10" s="26" customFormat="1" ht="15.6">
-      <c r="A16" s="121"/>
+      <c r="A16" s="122"/>
       <c r="B16" s="19" t="s">
         <v>62</v>
       </c>
@@ -6894,7 +6894,7 @@
       <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10" s="26" customFormat="1" ht="93.6">
-      <c r="A17" s="121"/>
+      <c r="A17" s="122"/>
       <c r="B17" s="19" t="s">
         <v>64</v>
       </c>
@@ -6914,7 +6914,7 @@
       <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10" s="26" customFormat="1" ht="93.6">
-      <c r="A18" s="121"/>
+      <c r="A18" s="122"/>
       <c r="B18" s="19" t="s">
         <v>66</v>
       </c>
@@ -6934,7 +6934,7 @@
       <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10" s="26" customFormat="1" ht="48" customHeight="1">
-      <c r="A19" s="121" t="s">
+      <c r="A19" s="122" t="s">
         <v>68</v>
       </c>
       <c r="B19" s="19" t="s">
@@ -6956,7 +6956,7 @@
       <c r="J19" s="33"/>
     </row>
     <row r="20" spans="1:10" s="26" customFormat="1" ht="78">
-      <c r="A20" s="121"/>
+      <c r="A20" s="122"/>
       <c r="B20" s="19" t="s">
         <v>71</v>
       </c>
@@ -6976,7 +6976,7 @@
       <c r="J20" s="33"/>
     </row>
     <row r="21" spans="1:10" s="26" customFormat="1" ht="46.8">
-      <c r="A21" s="121"/>
+      <c r="A21" s="122"/>
       <c r="B21" s="19" t="s">
         <v>73</v>
       </c>
@@ -6996,7 +6996,7 @@
       <c r="J21" s="33"/>
     </row>
     <row r="22" spans="1:10" s="26" customFormat="1" ht="62.4">
-      <c r="A22" s="121"/>
+      <c r="A22" s="122"/>
       <c r="B22" s="19" t="s">
         <v>75</v>
       </c>
@@ -7016,7 +7016,7 @@
       <c r="J22" s="33"/>
     </row>
     <row r="23" spans="1:10" s="26" customFormat="1" ht="48" customHeight="1">
-      <c r="A23" s="121" t="s">
+      <c r="A23" s="122" t="s">
         <v>77</v>
       </c>
       <c r="B23" s="19" t="s">
@@ -7038,7 +7038,7 @@
       <c r="J23" s="33"/>
     </row>
     <row r="24" spans="1:10" s="26" customFormat="1" ht="46.8">
-      <c r="A24" s="121"/>
+      <c r="A24" s="122"/>
       <c r="B24" s="19" t="s">
         <v>80</v>
       </c>
@@ -7058,7 +7058,7 @@
       <c r="J24" s="33"/>
     </row>
     <row r="25" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A25" s="121"/>
+      <c r="A25" s="122"/>
       <c r="B25" s="19" t="s">
         <v>82</v>
       </c>
@@ -7078,7 +7078,7 @@
       <c r="J25" s="33"/>
     </row>
     <row r="26" spans="1:10" s="26" customFormat="1" ht="46.8">
-      <c r="A26" s="121"/>
+      <c r="A26" s="122"/>
       <c r="B26" s="19" t="s">
         <v>84</v>
       </c>
@@ -7098,7 +7098,7 @@
       <c r="J26" s="33"/>
     </row>
     <row r="27" spans="1:10" s="26" customFormat="1" ht="48" customHeight="1">
-      <c r="A27" s="121" t="s">
+      <c r="A27" s="122" t="s">
         <v>86</v>
       </c>
       <c r="B27" s="19" t="s">
@@ -7120,7 +7120,7 @@
       <c r="J27" s="33"/>
     </row>
     <row r="28" spans="1:10" s="26" customFormat="1" ht="62.4">
-      <c r="A28" s="121"/>
+      <c r="A28" s="122"/>
       <c r="B28" s="19" t="s">
         <v>89</v>
       </c>
@@ -7138,7 +7138,7 @@
       <c r="J28" s="33"/>
     </row>
     <row r="29" spans="1:10" s="26" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A29" s="121" t="s">
+      <c r="A29" s="122" t="s">
         <v>91</v>
       </c>
       <c r="B29" s="19" t="s">
@@ -7158,7 +7158,7 @@
       <c r="J29" s="33"/>
     </row>
     <row r="30" spans="1:10" s="26" customFormat="1" ht="78">
-      <c r="A30" s="121"/>
+      <c r="A30" s="122"/>
       <c r="B30" s="19" t="s">
         <v>94</v>
       </c>
@@ -7176,7 +7176,7 @@
       <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" s="26" customFormat="1" ht="79.5" customHeight="1">
-      <c r="A31" s="121" t="s">
+      <c r="A31" s="122" t="s">
         <v>96</v>
       </c>
       <c r="B31" s="19" t="s">
@@ -7198,7 +7198,7 @@
       <c r="J31" s="33"/>
     </row>
     <row r="32" spans="1:10" s="26" customFormat="1" ht="62.4">
-      <c r="A32" s="121"/>
+      <c r="A32" s="122"/>
       <c r="B32" s="19" t="s">
         <v>99</v>
       </c>
@@ -7240,7 +7240,7 @@
       <c r="J33" s="33"/>
     </row>
     <row r="34" spans="1:10" s="26" customFormat="1" ht="48" customHeight="1">
-      <c r="A34" s="121" t="s">
+      <c r="A34" s="122" t="s">
         <v>104</v>
       </c>
       <c r="B34" s="19" t="s">
@@ -7262,7 +7262,7 @@
       <c r="J34" s="33"/>
     </row>
     <row r="35" spans="1:10" s="26" customFormat="1" ht="46.8">
-      <c r="A35" s="121"/>
+      <c r="A35" s="122"/>
       <c r="B35" s="19" t="s">
         <v>107</v>
       </c>
@@ -7282,7 +7282,7 @@
       <c r="J35" s="33"/>
     </row>
     <row r="36" spans="1:10" s="26" customFormat="1" ht="62.4">
-      <c r="A36" s="121"/>
+      <c r="A36" s="122"/>
       <c r="B36" s="19" t="s">
         <v>109</v>
       </c>
@@ -7302,7 +7302,7 @@
       <c r="J36" s="33"/>
     </row>
     <row r="37" spans="1:10" s="26" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A37" s="121" t="s">
+      <c r="A37" s="122" t="s">
         <v>111</v>
       </c>
       <c r="B37" s="19" t="s">
@@ -7326,7 +7326,7 @@
       <c r="J37" s="33"/>
     </row>
     <row r="38" spans="1:10" s="26" customFormat="1" ht="93.6">
-      <c r="A38" s="121"/>
+      <c r="A38" s="122"/>
       <c r="B38" s="19" t="s">
         <v>114</v>
       </c>
@@ -7364,7 +7364,7 @@
       <c r="J39" s="33"/>
     </row>
     <row r="40" spans="1:10" s="26" customFormat="1" ht="58.8" customHeight="1">
-      <c r="A40" s="121" t="s">
+      <c r="A40" s="122" t="s">
         <v>117</v>
       </c>
       <c r="B40" s="19" t="s">
@@ -7386,7 +7386,7 @@
       <c r="J40" s="33"/>
     </row>
     <row r="41" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A41" s="121"/>
+      <c r="A41" s="122"/>
       <c r="B41" s="19" t="s">
         <v>120</v>
       </c>
@@ -7406,7 +7406,7 @@
       <c r="J41" s="33"/>
     </row>
     <row r="42" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A42" s="121"/>
+      <c r="A42" s="122"/>
       <c r="B42" s="19" t="s">
         <v>122</v>
       </c>
@@ -7426,7 +7426,7 @@
       <c r="J42" s="33"/>
     </row>
     <row r="43" spans="1:10" s="26" customFormat="1" ht="62.4">
-      <c r="A43" s="121"/>
+      <c r="A43" s="122"/>
       <c r="B43" s="19" t="s">
         <v>124</v>
       </c>
@@ -7444,7 +7444,7 @@
       <c r="J43" s="33"/>
     </row>
     <row r="44" spans="1:10" s="26" customFormat="1" ht="93.6">
-      <c r="A44" s="121"/>
+      <c r="A44" s="122"/>
       <c r="B44" s="19" t="s">
         <v>126</v>
       </c>
@@ -7464,7 +7464,7 @@
       <c r="J44" s="33"/>
     </row>
     <row r="45" spans="1:10" s="26" customFormat="1" ht="62.4">
-      <c r="A45" s="121"/>
+      <c r="A45" s="122"/>
       <c r="B45" s="19" t="s">
         <v>128</v>
       </c>
@@ -7485,17 +7485,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A26"/>
     <mergeCell ref="A40:A45"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A30"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A23:A26"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="G2:G45" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -7567,7 +7567,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="26" customFormat="1" ht="48" customHeight="1">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="123" t="s">
         <v>130</v>
       </c>
       <c r="B2" s="45" t="s">
@@ -7595,7 +7595,7 @@
       <c r="J2" s="52"/>
     </row>
     <row r="3" spans="1:10" s="26" customFormat="1" ht="46.8">
-      <c r="A3" s="122"/>
+      <c r="A3" s="123"/>
       <c r="B3" s="45" t="s">
         <v>134</v>
       </c>
@@ -7621,7 +7621,7 @@
       <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" s="26" customFormat="1" ht="46.8">
-      <c r="A4" s="122"/>
+      <c r="A4" s="123"/>
       <c r="B4" s="45" t="s">
         <v>136</v>
       </c>
@@ -7647,7 +7647,7 @@
       <c r="J4" s="32"/>
     </row>
     <row r="5" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A5" s="122"/>
+      <c r="A5" s="123"/>
       <c r="B5" s="45" t="s">
         <v>138</v>
       </c>
@@ -7673,7 +7673,7 @@
       <c r="J5" s="32"/>
     </row>
     <row r="6" spans="1:10" s="26" customFormat="1" ht="15.6">
-      <c r="A6" s="122"/>
+      <c r="A6" s="123"/>
       <c r="B6" s="45" t="s">
         <v>140</v>
       </c>
@@ -7699,7 +7699,7 @@
       <c r="J6" s="32"/>
     </row>
     <row r="7" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A7" s="122"/>
+      <c r="A7" s="123"/>
       <c r="B7" s="45" t="s">
         <v>142</v>
       </c>
@@ -7725,7 +7725,7 @@
       <c r="J7" s="32"/>
     </row>
     <row r="8" spans="1:10" s="26" customFormat="1" ht="140.4">
-      <c r="A8" s="122"/>
+      <c r="A8" s="123"/>
       <c r="B8" s="45" t="s">
         <v>144</v>
       </c>
@@ -7751,7 +7751,7 @@
       <c r="J8" s="32"/>
     </row>
     <row r="9" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A9" s="122"/>
+      <c r="A9" s="123"/>
       <c r="B9" s="45" t="s">
         <v>146</v>
       </c>
@@ -7777,7 +7777,7 @@
       <c r="J9" s="32"/>
     </row>
     <row r="10" spans="1:10" s="26" customFormat="1" ht="62.4">
-      <c r="A10" s="122"/>
+      <c r="A10" s="123"/>
       <c r="B10" s="45" t="s">
         <v>148</v>
       </c>
@@ -7803,7 +7803,7 @@
       <c r="J10" s="32"/>
     </row>
     <row r="11" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A11" s="122"/>
+      <c r="A11" s="123"/>
       <c r="B11" s="45" t="s">
         <v>150</v>
       </c>
@@ -7829,7 +7829,7 @@
       <c r="J11" s="32"/>
     </row>
     <row r="12" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A12" s="122"/>
+      <c r="A12" s="123"/>
       <c r="B12" s="45" t="s">
         <v>152</v>
       </c>
@@ -7855,7 +7855,7 @@
       <c r="J12" s="32"/>
     </row>
     <row r="13" spans="1:10" s="26" customFormat="1" ht="46.8">
-      <c r="A13" s="122"/>
+      <c r="A13" s="123"/>
       <c r="B13" s="45" t="s">
         <v>154</v>
       </c>
@@ -7881,7 +7881,7 @@
       <c r="J13" s="32"/>
     </row>
     <row r="14" spans="1:10" s="26" customFormat="1" ht="111" customHeight="1">
-      <c r="A14" s="122" t="s">
+      <c r="A14" s="123" t="s">
         <v>156</v>
       </c>
       <c r="B14" s="45" t="s">
@@ -7909,7 +7909,7 @@
       <c r="J14" s="32"/>
     </row>
     <row r="15" spans="1:10" s="26" customFormat="1" ht="78">
-      <c r="A15" s="122"/>
+      <c r="A15" s="123"/>
       <c r="B15" s="45" t="s">
         <v>160</v>
       </c>
@@ -7935,7 +7935,7 @@
       <c r="J15" s="32"/>
     </row>
     <row r="16" spans="1:10" s="26" customFormat="1" ht="93.6">
-      <c r="A16" s="122"/>
+      <c r="A16" s="123"/>
       <c r="B16" s="45" t="s">
         <v>163</v>
       </c>
@@ -7959,7 +7959,7 @@
       <c r="J16" s="32"/>
     </row>
     <row r="17" spans="1:10" s="26" customFormat="1" ht="62.4">
-      <c r="A17" s="122"/>
+      <c r="A17" s="123"/>
       <c r="B17" s="45" t="s">
         <v>165</v>
       </c>
@@ -7985,7 +7985,7 @@
       <c r="J17" s="32"/>
     </row>
     <row r="18" spans="1:10" s="26" customFormat="1" ht="46.8">
-      <c r="A18" s="122"/>
+      <c r="A18" s="123"/>
       <c r="B18" s="45" t="s">
         <v>168</v>
       </c>
@@ -8011,7 +8011,7 @@
       <c r="J18" s="32"/>
     </row>
     <row r="19" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A19" s="122"/>
+      <c r="A19" s="123"/>
       <c r="B19" s="45" t="s">
         <v>171</v>
       </c>
@@ -8037,7 +8037,7 @@
       <c r="J19" s="32"/>
     </row>
     <row r="20" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A20" s="122"/>
+      <c r="A20" s="123"/>
       <c r="B20" s="45" t="s">
         <v>174</v>
       </c>
@@ -8063,7 +8063,7 @@
       <c r="J20" s="32"/>
     </row>
     <row r="21" spans="1:10" s="26" customFormat="1" ht="79.5" customHeight="1">
-      <c r="A21" s="122" t="s">
+      <c r="A21" s="123" t="s">
         <v>177</v>
       </c>
       <c r="B21" s="45" t="s">
@@ -8091,7 +8091,7 @@
       <c r="J21" s="32"/>
     </row>
     <row r="22" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A22" s="122"/>
+      <c r="A22" s="123"/>
       <c r="B22" s="45" t="s">
         <v>181</v>
       </c>
@@ -8117,7 +8117,7 @@
       <c r="J22" s="32"/>
     </row>
     <row r="23" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A23" s="122"/>
+      <c r="A23" s="123"/>
       <c r="B23" s="45" t="s">
         <v>184</v>
       </c>
@@ -8143,7 +8143,7 @@
       <c r="J23" s="32"/>
     </row>
     <row r="24" spans="1:10" s="26" customFormat="1" ht="95.25" customHeight="1">
-      <c r="A24" s="122" t="s">
+      <c r="A24" s="123" t="s">
         <v>187</v>
       </c>
       <c r="B24" s="45" t="s">
@@ -8171,7 +8171,7 @@
       <c r="J24" s="32"/>
     </row>
     <row r="25" spans="1:10" s="26" customFormat="1" ht="62.4">
-      <c r="A25" s="122"/>
+      <c r="A25" s="123"/>
       <c r="B25" s="45" t="s">
         <v>190</v>
       </c>
@@ -8197,7 +8197,7 @@
       <c r="J25" s="32"/>
     </row>
     <row r="26" spans="1:10" s="26" customFormat="1" ht="62.4">
-      <c r="A26" s="122"/>
+      <c r="A26" s="123"/>
       <c r="B26" s="45" t="s">
         <v>192</v>
       </c>
@@ -8223,7 +8223,7 @@
       <c r="J26" s="32"/>
     </row>
     <row r="27" spans="1:10" s="26" customFormat="1" ht="46.8">
-      <c r="A27" s="122"/>
+      <c r="A27" s="123"/>
       <c r="B27" s="45" t="s">
         <v>194</v>
       </c>
@@ -8249,7 +8249,7 @@
       <c r="J27" s="32"/>
     </row>
     <row r="28" spans="1:10" s="26" customFormat="1" ht="109.2">
-      <c r="A28" s="122"/>
+      <c r="A28" s="123"/>
       <c r="B28" s="45" t="s">
         <v>196</v>
       </c>
@@ -8275,7 +8275,7 @@
       <c r="J28" s="33"/>
     </row>
     <row r="29" spans="1:10" s="26" customFormat="1" ht="48" customHeight="1">
-      <c r="A29" s="122" t="s">
+      <c r="A29" s="123" t="s">
         <v>198</v>
       </c>
       <c r="B29" s="45" t="s">
@@ -8303,7 +8303,7 @@
       <c r="J29" s="33"/>
     </row>
     <row r="30" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A30" s="122"/>
+      <c r="A30" s="123"/>
       <c r="B30" s="45" t="s">
         <v>201</v>
       </c>
@@ -8329,7 +8329,7 @@
       <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" s="26" customFormat="1" ht="46.8">
-      <c r="A31" s="122"/>
+      <c r="A31" s="123"/>
       <c r="B31" s="45" t="s">
         <v>203</v>
       </c>
@@ -8355,7 +8355,7 @@
       <c r="J31" s="33"/>
     </row>
     <row r="32" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A32" s="122"/>
+      <c r="A32" s="123"/>
       <c r="B32" s="45" t="s">
         <v>205</v>
       </c>
@@ -8381,7 +8381,7 @@
       <c r="J32" s="33"/>
     </row>
     <row r="33" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A33" s="122"/>
+      <c r="A33" s="123"/>
       <c r="B33" s="45" t="s">
         <v>207</v>
       </c>
@@ -8407,7 +8407,7 @@
       <c r="J33" s="33"/>
     </row>
     <row r="34" spans="1:10" s="26" customFormat="1" ht="62.4">
-      <c r="A34" s="122"/>
+      <c r="A34" s="123"/>
       <c r="B34" s="45" t="s">
         <v>210</v>
       </c>
@@ -8433,7 +8433,7 @@
       <c r="J34" s="33"/>
     </row>
     <row r="35" spans="1:10" s="26" customFormat="1" ht="46.8">
-      <c r="A35" s="122"/>
+      <c r="A35" s="123"/>
       <c r="B35" s="45" t="s">
         <v>212</v>
       </c>
@@ -8459,7 +8459,7 @@
       <c r="J35" s="33"/>
     </row>
     <row r="36" spans="1:10" s="26" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A36" s="122" t="s">
+      <c r="A36" s="123" t="s">
         <v>214</v>
       </c>
       <c r="B36" s="45" t="s">
@@ -8487,7 +8487,7 @@
       <c r="J36" s="33"/>
     </row>
     <row r="37" spans="1:10" s="26" customFormat="1" ht="46.8">
-      <c r="A37" s="122"/>
+      <c r="A37" s="123"/>
       <c r="B37" s="45" t="s">
         <v>218</v>
       </c>
@@ -8513,7 +8513,7 @@
       <c r="J37" s="33"/>
     </row>
     <row r="38" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A38" s="122"/>
+      <c r="A38" s="123"/>
       <c r="B38" s="45" t="s">
         <v>220</v>
       </c>
@@ -8539,7 +8539,7 @@
       <c r="J38" s="33"/>
     </row>
     <row r="39" spans="1:10" s="26" customFormat="1" ht="48" customHeight="1">
-      <c r="A39" s="122" t="s">
+      <c r="A39" s="123" t="s">
         <v>222</v>
       </c>
       <c r="B39" s="45" t="s">
@@ -8567,7 +8567,7 @@
       <c r="J39" s="33"/>
     </row>
     <row r="40" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A40" s="122"/>
+      <c r="A40" s="123"/>
       <c r="B40" s="45" t="s">
         <v>226</v>
       </c>
@@ -8593,7 +8593,7 @@
       <c r="J40" s="33"/>
     </row>
     <row r="41" spans="1:10" s="26" customFormat="1" ht="46.8">
-      <c r="A41" s="122"/>
+      <c r="A41" s="123"/>
       <c r="B41" s="45" t="s">
         <v>228</v>
       </c>
@@ -8619,7 +8619,7 @@
       <c r="J41" s="33"/>
     </row>
     <row r="42" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A42" s="122"/>
+      <c r="A42" s="123"/>
       <c r="B42" s="45" t="s">
         <v>230</v>
       </c>
@@ -8645,7 +8645,7 @@
       <c r="J42" s="33"/>
     </row>
     <row r="43" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A43" s="122"/>
+      <c r="A43" s="123"/>
       <c r="B43" s="45" t="s">
         <v>232</v>
       </c>
@@ -8671,7 +8671,7 @@
       <c r="J43" s="33"/>
     </row>
     <row r="44" spans="1:10" s="26" customFormat="1" ht="46.8">
-      <c r="A44" s="122"/>
+      <c r="A44" s="123"/>
       <c r="B44" s="45" t="s">
         <v>234</v>
       </c>
@@ -8697,7 +8697,7 @@
       <c r="J44" s="33"/>
     </row>
     <row r="45" spans="1:10" s="26" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A45" s="122" t="s">
+      <c r="A45" s="123" t="s">
         <v>236</v>
       </c>
       <c r="B45" s="45" t="s">
@@ -8725,7 +8725,7 @@
       <c r="J45" s="33"/>
     </row>
     <row r="46" spans="1:10" s="26" customFormat="1" ht="46.8">
-      <c r="A46" s="122"/>
+      <c r="A46" s="123"/>
       <c r="B46" s="45" t="s">
         <v>240</v>
       </c>
@@ -8751,7 +8751,7 @@
       <c r="J46" s="33"/>
     </row>
     <row r="47" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A47" s="122"/>
+      <c r="A47" s="123"/>
       <c r="B47" s="45" t="s">
         <v>242</v>
       </c>
@@ -8777,7 +8777,7 @@
       <c r="J47" s="33"/>
     </row>
     <row r="48" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A48" s="122"/>
+      <c r="A48" s="123"/>
       <c r="B48" s="45" t="s">
         <v>244</v>
       </c>
@@ -8803,7 +8803,7 @@
       <c r="J48" s="33"/>
     </row>
     <row r="49" spans="1:10" s="26" customFormat="1" ht="46.8">
-      <c r="A49" s="122"/>
+      <c r="A49" s="123"/>
       <c r="B49" s="45" t="s">
         <v>246</v>
       </c>
@@ -8829,7 +8829,7 @@
       <c r="J49" s="33"/>
     </row>
     <row r="50" spans="1:10" s="26" customFormat="1" ht="46.8">
-      <c r="A50" s="122"/>
+      <c r="A50" s="123"/>
       <c r="B50" s="45" t="s">
         <v>249</v>
       </c>
@@ -8855,7 +8855,7 @@
       <c r="J50" s="33"/>
     </row>
     <row r="51" spans="1:10" s="26" customFormat="1" ht="46.8">
-      <c r="A51" s="122"/>
+      <c r="A51" s="123"/>
       <c r="B51" s="45" t="s">
         <v>252</v>
       </c>
@@ -8881,7 +8881,7 @@
       <c r="J51" s="33"/>
     </row>
     <row r="52" spans="1:10" s="26" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A52" s="122" t="s">
+      <c r="A52" s="123" t="s">
         <v>255</v>
       </c>
       <c r="B52" s="45" t="s">
@@ -8909,7 +8909,7 @@
       <c r="J52" s="33"/>
     </row>
     <row r="53" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A53" s="122"/>
+      <c r="A53" s="123"/>
       <c r="B53" s="45" t="s">
         <v>259</v>
       </c>
@@ -8935,7 +8935,7 @@
       <c r="J53" s="33"/>
     </row>
     <row r="54" spans="1:10" s="26" customFormat="1" ht="31.2">
-      <c r="A54" s="122"/>
+      <c r="A54" s="123"/>
       <c r="B54" s="45" t="s">
         <v>261</v>
       </c>
@@ -8961,7 +8961,7 @@
       <c r="J54" s="33"/>
     </row>
     <row r="55" spans="1:10" s="26" customFormat="1" ht="79.5" customHeight="1">
-      <c r="A55" s="122" t="s">
+      <c r="A55" s="123" t="s">
         <v>263</v>
       </c>
       <c r="B55" s="45" t="s">
@@ -8989,7 +8989,7 @@
       <c r="J55" s="33"/>
     </row>
     <row r="56" spans="1:10" s="26" customFormat="1" ht="46.8">
-      <c r="A56" s="122"/>
+      <c r="A56" s="123"/>
       <c r="B56" s="45" t="s">
         <v>268</v>
       </c>
@@ -9015,7 +9015,7 @@
       <c r="J56" s="33"/>
     </row>
     <row r="57" spans="1:10" s="26" customFormat="1" ht="46.8">
-      <c r="A57" s="122"/>
+      <c r="A57" s="123"/>
       <c r="B57" s="45" t="s">
         <v>270</v>
       </c>
@@ -9041,7 +9041,7 @@
       <c r="J57" s="33"/>
     </row>
     <row r="58" spans="1:10" s="26" customFormat="1" ht="93.6">
-      <c r="A58" s="122"/>
+      <c r="A58" s="123"/>
       <c r="B58" s="45" t="s">
         <v>272</v>
       </c>
@@ -9066,16 +9066,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="A14:A20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="A29:A35"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A39:A44"/>
     <mergeCell ref="A45:A51"/>
     <mergeCell ref="A52:A54"/>
     <mergeCell ref="A55:A58"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="A14:A20"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="A29:A35"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="G2:G58" xr:uid="{00000000-0002-0000-0200-000000000000}">
@@ -9169,7 +9169,7 @@
       <c r="J2" s="66"/>
     </row>
     <row r="3" spans="1:10" ht="63.75" customHeight="1">
-      <c r="A3" s="122" t="s">
+      <c r="A3" s="123" t="s">
         <v>277</v>
       </c>
       <c r="B3" s="63" t="s">
@@ -9193,7 +9193,7 @@
       <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:10" ht="46.8">
-      <c r="A4" s="122"/>
+      <c r="A4" s="123"/>
       <c r="B4" s="63" t="s">
         <v>280</v>
       </c>
@@ -9215,7 +9215,7 @@
       <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="46.8">
-      <c r="A5" s="122"/>
+      <c r="A5" s="123"/>
       <c r="B5" s="63" t="s">
         <v>282</v>
       </c>
@@ -9237,7 +9237,7 @@
       <c r="J5" s="33"/>
     </row>
     <row r="6" spans="1:10" ht="62.4">
-      <c r="A6" s="122"/>
+      <c r="A6" s="123"/>
       <c r="B6" s="63" t="s">
         <v>284</v>
       </c>
@@ -9259,7 +9259,7 @@
       <c r="J6" s="33"/>
     </row>
     <row r="7" spans="1:10" ht="79.5" customHeight="1">
-      <c r="A7" s="122" t="s">
+      <c r="A7" s="123" t="s">
         <v>286</v>
       </c>
       <c r="B7" s="63" t="s">
@@ -9283,7 +9283,7 @@
       <c r="J7" s="33"/>
     </row>
     <row r="8" spans="1:10" ht="109.2">
-      <c r="A8" s="122"/>
+      <c r="A8" s="123"/>
       <c r="B8" s="63" t="s">
         <v>289</v>
       </c>
@@ -9305,7 +9305,7 @@
       <c r="J8" s="33"/>
     </row>
     <row r="9" spans="1:10" ht="62.4">
-      <c r="A9" s="122"/>
+      <c r="A9" s="123"/>
       <c r="B9" s="63" t="s">
         <v>291</v>
       </c>
@@ -9325,7 +9325,7 @@
       <c r="J9" s="33"/>
     </row>
     <row r="10" spans="1:10" ht="31.2">
-      <c r="A10" s="122"/>
+      <c r="A10" s="123"/>
       <c r="B10" s="63" t="s">
         <v>293</v>
       </c>
@@ -9347,7 +9347,7 @@
       <c r="J10" s="33"/>
     </row>
     <row r="11" spans="1:10" ht="48" customHeight="1">
-      <c r="A11" s="122" t="s">
+      <c r="A11" s="123" t="s">
         <v>295</v>
       </c>
       <c r="B11" s="63" t="s">
@@ -9371,7 +9371,7 @@
       <c r="J11" s="33"/>
     </row>
     <row r="12" spans="1:10" ht="46.8">
-      <c r="A12" s="122"/>
+      <c r="A12" s="123"/>
       <c r="B12" s="63" t="s">
         <v>299</v>
       </c>
@@ -9393,7 +9393,7 @@
       <c r="J12" s="33"/>
     </row>
     <row r="13" spans="1:10" ht="62.4">
-      <c r="A13" s="122"/>
+      <c r="A13" s="123"/>
       <c r="B13" s="63" t="s">
         <v>301</v>
       </c>
@@ -9415,7 +9415,7 @@
       <c r="J13" s="33"/>
     </row>
     <row r="14" spans="1:10" ht="31.2">
-      <c r="A14" s="122"/>
+      <c r="A14" s="123"/>
       <c r="B14" s="63" t="s">
         <v>303</v>
       </c>
@@ -9437,7 +9437,7 @@
       <c r="J14" s="33"/>
     </row>
     <row r="15" spans="1:10" ht="93.6">
-      <c r="A15" s="122"/>
+      <c r="A15" s="123"/>
       <c r="B15" s="63" t="s">
         <v>305</v>
       </c>
@@ -9459,7 +9459,7 @@
       <c r="J15" s="33"/>
     </row>
     <row r="16" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A16" s="122" t="s">
+      <c r="A16" s="123" t="s">
         <v>307</v>
       </c>
       <c r="B16" s="63" t="s">
@@ -9483,7 +9483,7 @@
       <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10" ht="31.2">
-      <c r="A17" s="122"/>
+      <c r="A17" s="123"/>
       <c r="B17" s="63" t="s">
         <v>311</v>
       </c>
@@ -9503,7 +9503,7 @@
       <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10" ht="46.8">
-      <c r="A18" s="122"/>
+      <c r="A18" s="123"/>
       <c r="B18" s="63" t="s">
         <v>313</v>
       </c>
@@ -9523,7 +9523,7 @@
       <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10" ht="63.75" customHeight="1">
-      <c r="A19" s="122" t="s">
+      <c r="A19" s="123" t="s">
         <v>315</v>
       </c>
       <c r="B19" s="63" t="s">
@@ -9547,7 +9547,7 @@
       <c r="J19" s="33"/>
     </row>
     <row r="20" spans="1:10" ht="46.8">
-      <c r="A20" s="122"/>
+      <c r="A20" s="123"/>
       <c r="B20" s="63" t="s">
         <v>319</v>
       </c>
@@ -9626,8 +9626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMJ11"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="21"/>
@@ -9677,7 +9677,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="48" customHeight="1">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="123" t="s">
         <v>324</v>
       </c>
       <c r="B2" s="78" t="s">
@@ -9693,13 +9693,15 @@
       <c r="F2" s="49" t="s">
         <v>326</v>
       </c>
-      <c r="G2" s="50"/>
+      <c r="G2" s="50" t="s">
+        <v>26</v>
+      </c>
       <c r="H2" s="50"/>
       <c r="I2" s="50"/>
       <c r="J2" s="66"/>
     </row>
     <row r="3" spans="1:10" ht="46.8">
-      <c r="A3" s="122"/>
+      <c r="A3" s="123"/>
       <c r="B3" s="78" t="s">
         <v>327</v>
       </c>
@@ -9713,13 +9715,15 @@
       <c r="F3" s="30" t="s">
         <v>328</v>
       </c>
-      <c r="G3" s="29"/>
+      <c r="G3" s="29" t="s">
+        <v>26</v>
+      </c>
       <c r="H3" s="29"/>
       <c r="I3" s="29"/>
       <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:10" ht="93.6">
-      <c r="A4" s="122"/>
+      <c r="A4" s="123"/>
       <c r="B4" s="78" t="s">
         <v>329</v>
       </c>
@@ -9733,13 +9737,15 @@
       <c r="F4" s="30" t="s">
         <v>330</v>
       </c>
-      <c r="G4" s="29"/>
+      <c r="G4" s="29" t="s">
+        <v>26</v>
+      </c>
       <c r="H4" s="29"/>
       <c r="I4" s="29"/>
       <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="15.6">
-      <c r="A5" s="122"/>
+      <c r="A5" s="123"/>
       <c r="B5" s="78" t="s">
         <v>331</v>
       </c>
@@ -9761,7 +9767,7 @@
       <c r="J5" s="33"/>
     </row>
     <row r="6" spans="1:10" ht="46.8">
-      <c r="A6" s="122"/>
+      <c r="A6" s="123"/>
       <c r="B6" s="78" t="s">
         <v>332</v>
       </c>
@@ -9775,13 +9781,15 @@
       <c r="F6" s="30" t="s">
         <v>333</v>
       </c>
-      <c r="G6" s="29"/>
+      <c r="G6" s="29" t="s">
+        <v>26</v>
+      </c>
       <c r="H6" s="29"/>
       <c r="I6" s="29"/>
       <c r="J6" s="33"/>
     </row>
     <row r="7" spans="1:10" ht="79.5" customHeight="1">
-      <c r="A7" s="122" t="s">
+      <c r="A7" s="123" t="s">
         <v>334</v>
       </c>
       <c r="B7" s="78" t="s">
@@ -9797,13 +9805,15 @@
       <c r="F7" s="30" t="s">
         <v>336</v>
       </c>
-      <c r="G7" s="29"/>
+      <c r="G7" s="29" t="s">
+        <v>26</v>
+      </c>
       <c r="H7" s="29"/>
       <c r="I7" s="29"/>
       <c r="J7" s="33"/>
     </row>
     <row r="8" spans="1:10" ht="46.8">
-      <c r="A8" s="122"/>
+      <c r="A8" s="123"/>
       <c r="B8" s="78" t="s">
         <v>337</v>
       </c>
@@ -9817,13 +9827,15 @@
       <c r="F8" s="30" t="s">
         <v>338</v>
       </c>
-      <c r="G8" s="29"/>
+      <c r="G8" s="29" t="s">
+        <v>26</v>
+      </c>
       <c r="H8" s="29"/>
       <c r="I8" s="29"/>
       <c r="J8" s="33"/>
     </row>
     <row r="9" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A9" s="122" t="s">
+      <c r="A9" s="123" t="s">
         <v>339</v>
       </c>
       <c r="B9" s="78" t="s">
@@ -9839,13 +9851,15 @@
       <c r="F9" s="30" t="s">
         <v>341</v>
       </c>
-      <c r="G9" s="29"/>
+      <c r="G9" s="29" t="s">
+        <v>26</v>
+      </c>
       <c r="H9" s="29"/>
       <c r="I9" s="29"/>
       <c r="J9" s="33"/>
     </row>
     <row r="10" spans="1:10" ht="62.4">
-      <c r="A10" s="122"/>
+      <c r="A10" s="123"/>
       <c r="B10" s="78" t="s">
         <v>342</v>
       </c>
@@ -9859,13 +9873,15 @@
       <c r="F10" s="30" t="s">
         <v>343</v>
       </c>
-      <c r="G10" s="29"/>
+      <c r="G10" s="29" t="s">
+        <v>26</v>
+      </c>
       <c r="H10" s="29"/>
       <c r="I10" s="29"/>
       <c r="J10" s="33"/>
     </row>
     <row r="11" spans="1:10" ht="62.4">
-      <c r="A11" s="122"/>
+      <c r="A11" s="123"/>
       <c r="B11" s="78" t="s">
         <v>344</v>
       </c>
@@ -9879,7 +9895,9 @@
       <c r="F11" s="37" t="s">
         <v>345</v>
       </c>
-      <c r="G11" s="36"/>
+      <c r="G11" s="36" t="s">
+        <v>26</v>
+      </c>
       <c r="H11" s="36"/>
       <c r="I11" s="36"/>
       <c r="J11" s="38"/>
@@ -9959,7 +9977,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="79.5" customHeight="1">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="123" t="s">
         <v>346</v>
       </c>
       <c r="B2" s="63" t="s">
@@ -9983,7 +10001,7 @@
       <c r="J2" s="66"/>
     </row>
     <row r="3" spans="1:10" ht="93.6">
-      <c r="A3" s="122"/>
+      <c r="A3" s="123"/>
       <c r="B3" s="63" t="s">
         <v>349</v>
       </c>
@@ -10005,7 +10023,7 @@
       <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:10" ht="78">
-      <c r="A4" s="122"/>
+      <c r="A4" s="123"/>
       <c r="B4" s="63" t="s">
         <v>351</v>
       </c>
@@ -10027,7 +10045,7 @@
       <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="109.2">
-      <c r="A5" s="122"/>
+      <c r="A5" s="123"/>
       <c r="B5" s="63" t="s">
         <v>353</v>
       </c>
@@ -10049,7 +10067,7 @@
       <c r="J5" s="33"/>
     </row>
     <row r="6" spans="1:10" ht="46.8">
-      <c r="A6" s="122"/>
+      <c r="A6" s="123"/>
       <c r="B6" s="63" t="s">
         <v>355</v>
       </c>
@@ -10071,7 +10089,7 @@
       <c r="J6" s="33"/>
     </row>
     <row r="7" spans="1:10" ht="63.75" customHeight="1">
-      <c r="A7" s="122" t="s">
+      <c r="A7" s="123" t="s">
         <v>357</v>
       </c>
       <c r="B7" s="63" t="s">
@@ -10095,7 +10113,7 @@
       <c r="J7" s="33"/>
     </row>
     <row r="8" spans="1:10" ht="31.2">
-      <c r="A8" s="122"/>
+      <c r="A8" s="123"/>
       <c r="B8" s="63" t="s">
         <v>359</v>
       </c>
@@ -10117,7 +10135,7 @@
       <c r="J8" s="33"/>
     </row>
     <row r="9" spans="1:10" ht="31.2">
-      <c r="A9" s="122"/>
+      <c r="A9" s="123"/>
       <c r="B9" s="63" t="s">
         <v>253</v>
       </c>
@@ -10139,7 +10157,7 @@
       <c r="J9" s="33"/>
     </row>
     <row r="10" spans="1:10" ht="62.4">
-      <c r="A10" s="122"/>
+      <c r="A10" s="123"/>
       <c r="B10" s="63" t="s">
         <v>362</v>
       </c>
@@ -10161,7 +10179,7 @@
       <c r="J10" s="33"/>
     </row>
     <row r="11" spans="1:10" ht="46.8">
-      <c r="A11" s="122"/>
+      <c r="A11" s="123"/>
       <c r="B11" s="63" t="s">
         <v>166</v>
       </c>
@@ -10183,7 +10201,7 @@
       <c r="J11" s="33"/>
     </row>
     <row r="12" spans="1:10" ht="62.4">
-      <c r="A12" s="122"/>
+      <c r="A12" s="123"/>
       <c r="B12" s="63" t="s">
         <v>169</v>
       </c>
@@ -10205,7 +10223,7 @@
       <c r="J12" s="33"/>
     </row>
     <row r="13" spans="1:10" ht="62.4">
-      <c r="A13" s="122"/>
+      <c r="A13" s="123"/>
       <c r="B13" s="63" t="s">
         <v>366</v>
       </c>
@@ -10227,7 +10245,7 @@
       <c r="J13" s="33"/>
     </row>
     <row r="14" spans="1:10" ht="62.4">
-      <c r="A14" s="122"/>
+      <c r="A14" s="123"/>
       <c r="B14" s="63" t="s">
         <v>172</v>
       </c>
@@ -10249,7 +10267,7 @@
       <c r="J14" s="33"/>
     </row>
     <row r="15" spans="1:10" ht="126.75" customHeight="1">
-      <c r="A15" s="122" t="s">
+      <c r="A15" s="123" t="s">
         <v>369</v>
       </c>
       <c r="B15" s="63" t="s">
@@ -10273,7 +10291,7 @@
       <c r="J15" s="33"/>
     </row>
     <row r="16" spans="1:10" ht="78">
-      <c r="A16" s="122"/>
+      <c r="A16" s="123"/>
       <c r="B16" s="63" t="s">
         <v>372</v>
       </c>
@@ -10295,7 +10313,7 @@
       <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10" ht="62.4">
-      <c r="A17" s="122"/>
+      <c r="A17" s="123"/>
       <c r="B17" s="63" t="s">
         <v>374</v>
       </c>
@@ -10317,7 +10335,7 @@
       <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10" ht="78">
-      <c r="A18" s="122"/>
+      <c r="A18" s="123"/>
       <c r="B18" s="63" t="s">
         <v>376</v>
       </c>
@@ -10339,7 +10357,7 @@
       <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10" ht="93.6">
-      <c r="A19" s="122"/>
+      <c r="A19" s="123"/>
       <c r="B19" s="63" t="s">
         <v>378</v>
       </c>
@@ -10361,7 +10379,7 @@
       <c r="J19" s="33"/>
     </row>
     <row r="20" spans="1:10" ht="62.4">
-      <c r="A20" s="122"/>
+      <c r="A20" s="123"/>
       <c r="B20" s="63" t="s">
         <v>380</v>
       </c>
@@ -10383,7 +10401,7 @@
       <c r="J20" s="33"/>
     </row>
     <row r="21" spans="1:10" ht="78">
-      <c r="A21" s="122"/>
+      <c r="A21" s="123"/>
       <c r="B21" s="63" t="s">
         <v>382</v>
       </c>
@@ -10405,7 +10423,7 @@
       <c r="J21" s="33"/>
     </row>
     <row r="22" spans="1:10" ht="78">
-      <c r="A22" s="122"/>
+      <c r="A22" s="123"/>
       <c r="B22" s="63" t="s">
         <v>384</v>
       </c>
@@ -10427,7 +10445,7 @@
       <c r="J22" s="33"/>
     </row>
     <row r="23" spans="1:10" ht="31.2">
-      <c r="A23" s="122"/>
+      <c r="A23" s="123"/>
       <c r="B23" s="63" t="s">
         <v>386</v>
       </c>
@@ -10449,7 +10467,7 @@
       <c r="J23" s="33"/>
     </row>
     <row r="24" spans="1:10" ht="46.8">
-      <c r="A24" s="122"/>
+      <c r="A24" s="123"/>
       <c r="B24" s="63" t="s">
         <v>388</v>
       </c>
@@ -10471,7 +10489,7 @@
       <c r="J24" s="33"/>
     </row>
     <row r="25" spans="1:10" ht="48" customHeight="1">
-      <c r="A25" s="122" t="s">
+      <c r="A25" s="123" t="s">
         <v>390</v>
       </c>
       <c r="B25" s="63" t="s">
@@ -10495,7 +10513,7 @@
       <c r="J25" s="33"/>
     </row>
     <row r="26" spans="1:10" ht="31.2">
-      <c r="A26" s="122"/>
+      <c r="A26" s="123"/>
       <c r="B26" s="63" t="s">
         <v>393</v>
       </c>
@@ -10517,7 +10535,7 @@
       <c r="J26" s="33"/>
     </row>
     <row r="27" spans="1:10" ht="31.2">
-      <c r="A27" s="122"/>
+      <c r="A27" s="123"/>
       <c r="B27" s="63" t="s">
         <v>395</v>
       </c>
@@ -10539,7 +10557,7 @@
       <c r="J27" s="33"/>
     </row>
     <row r="28" spans="1:10" ht="63.75" customHeight="1">
-      <c r="A28" s="122" t="s">
+      <c r="A28" s="123" t="s">
         <v>397</v>
       </c>
       <c r="B28" s="63" t="s">
@@ -10563,7 +10581,7 @@
       <c r="J28" s="33"/>
     </row>
     <row r="29" spans="1:10" ht="62.4">
-      <c r="A29" s="122"/>
+      <c r="A29" s="123"/>
       <c r="B29" s="63" t="s">
         <v>400</v>
       </c>
@@ -10585,7 +10603,7 @@
       <c r="J29" s="33"/>
     </row>
     <row r="30" spans="1:10" ht="46.8">
-      <c r="A30" s="122"/>
+      <c r="A30" s="123"/>
       <c r="B30" s="63" t="s">
         <v>402</v>
       </c>
@@ -10607,7 +10625,7 @@
       <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="46.8">
-      <c r="A31" s="122"/>
+      <c r="A31" s="123"/>
       <c r="B31" s="63" t="s">
         <v>404</v>
       </c>
@@ -10629,7 +10647,7 @@
       <c r="J31" s="38"/>
     </row>
     <row r="32" spans="1:10">
-      <c r="G32" s="124"/>
+      <c r="G32" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -10709,7 +10727,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="48" customHeight="1">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="123" t="s">
         <v>406</v>
       </c>
       <c r="B2" s="63" t="s">
@@ -10731,7 +10749,7 @@
       <c r="J2" s="66"/>
     </row>
     <row r="3" spans="1:10" ht="31.2">
-      <c r="A3" s="122"/>
+      <c r="A3" s="123"/>
       <c r="B3" s="63" t="s">
         <v>409</v>
       </c>
@@ -10751,7 +10769,7 @@
       <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:10" ht="46.8">
-      <c r="A4" s="122"/>
+      <c r="A4" s="123"/>
       <c r="B4" s="63" t="s">
         <v>182</v>
       </c>
@@ -10771,7 +10789,7 @@
       <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A5" s="122" t="s">
+      <c r="A5" s="123" t="s">
         <v>412</v>
       </c>
       <c r="B5" s="63" t="s">
@@ -10793,7 +10811,7 @@
       <c r="J5" s="33"/>
     </row>
     <row r="6" spans="1:10" ht="46.8">
-      <c r="A6" s="122"/>
+      <c r="A6" s="123"/>
       <c r="B6" s="63" t="s">
         <v>415</v>
       </c>
@@ -10813,7 +10831,7 @@
       <c r="J6" s="33"/>
     </row>
     <row r="7" spans="1:10" ht="31.2">
-      <c r="A7" s="122"/>
+      <c r="A7" s="123"/>
       <c r="B7" s="63" t="s">
         <v>417</v>
       </c>
@@ -10833,7 +10851,7 @@
       <c r="J7" s="33"/>
     </row>
     <row r="8" spans="1:10" ht="46.8">
-      <c r="A8" s="122"/>
+      <c r="A8" s="123"/>
       <c r="B8" s="63" t="s">
         <v>419</v>
       </c>
@@ -10853,7 +10871,7 @@
       <c r="J8" s="33"/>
     </row>
     <row r="9" spans="1:10" ht="46.8">
-      <c r="A9" s="122"/>
+      <c r="A9" s="123"/>
       <c r="B9" s="63" t="s">
         <v>421</v>
       </c>
@@ -10873,7 +10891,7 @@
       <c r="J9" s="33"/>
     </row>
     <row r="10" spans="1:10" ht="46.8">
-      <c r="A10" s="122"/>
+      <c r="A10" s="123"/>
       <c r="B10" s="63" t="s">
         <v>423</v>
       </c>
@@ -10893,7 +10911,7 @@
       <c r="J10" s="33"/>
     </row>
     <row r="11" spans="1:10" ht="31.2">
-      <c r="A11" s="122"/>
+      <c r="A11" s="123"/>
       <c r="B11" s="63" t="s">
         <v>425</v>
       </c>
@@ -10913,7 +10931,7 @@
       <c r="J11" s="33"/>
     </row>
     <row r="12" spans="1:10" ht="31.2">
-      <c r="A12" s="122"/>
+      <c r="A12" s="123"/>
       <c r="B12" s="63" t="s">
         <v>427</v>
       </c>
@@ -10933,7 +10951,7 @@
       <c r="J12" s="33"/>
     </row>
     <row r="13" spans="1:10" ht="48" customHeight="1">
-      <c r="A13" s="122" t="s">
+      <c r="A13" s="123" t="s">
         <v>429</v>
       </c>
       <c r="B13" s="63" t="s">
@@ -10955,7 +10973,7 @@
       <c r="J13" s="33"/>
     </row>
     <row r="14" spans="1:10" ht="46.8">
-      <c r="A14" s="122"/>
+      <c r="A14" s="123"/>
       <c r="B14" s="63" t="s">
         <v>432</v>
       </c>
@@ -10975,7 +10993,7 @@
       <c r="J14" s="33"/>
     </row>
     <row r="15" spans="1:10" ht="31.2">
-      <c r="A15" s="122"/>
+      <c r="A15" s="123"/>
       <c r="B15" s="63" t="s">
         <v>434</v>
       </c>
@@ -10995,7 +11013,7 @@
       <c r="J15" s="33"/>
     </row>
     <row r="16" spans="1:10" ht="48" customHeight="1">
-      <c r="A16" s="122" t="s">
+      <c r="A16" s="123" t="s">
         <v>436</v>
       </c>
       <c r="B16" s="63" t="s">
@@ -11017,7 +11035,7 @@
       <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10" ht="46.8">
-      <c r="A17" s="122"/>
+      <c r="A17" s="123"/>
       <c r="B17" s="63" t="s">
         <v>439</v>
       </c>
@@ -11113,7 +11131,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="48" customHeight="1">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="123" t="s">
         <v>441</v>
       </c>
       <c r="B2" s="63" t="s">
@@ -11135,7 +11153,7 @@
       <c r="J2" s="94"/>
     </row>
     <row r="3" spans="1:10" ht="46.8">
-      <c r="A3" s="122"/>
+      <c r="A3" s="123"/>
       <c r="B3" s="63" t="s">
         <v>309</v>
       </c>
@@ -11155,7 +11173,7 @@
       <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:10" ht="62.4">
-      <c r="A4" s="122"/>
+      <c r="A4" s="123"/>
       <c r="B4" s="63" t="s">
         <v>444</v>
       </c>
@@ -11175,7 +11193,7 @@
       <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="46.8">
-      <c r="A5" s="122"/>
+      <c r="A5" s="123"/>
       <c r="B5" s="63" t="s">
         <v>446</v>
       </c>
@@ -11195,7 +11213,7 @@
       <c r="J5" s="33"/>
     </row>
     <row r="6" spans="1:10" ht="48" customHeight="1">
-      <c r="A6" s="122" t="s">
+      <c r="A6" s="123" t="s">
         <v>448</v>
       </c>
       <c r="B6" s="63" t="s">
@@ -11217,7 +11235,7 @@
       <c r="J6" s="33"/>
     </row>
     <row r="7" spans="1:10" ht="46.8">
-      <c r="A7" s="122"/>
+      <c r="A7" s="123"/>
       <c r="B7" s="63" t="s">
         <v>450</v>
       </c>
@@ -11237,7 +11255,7 @@
       <c r="J7" s="33"/>
     </row>
     <row r="8" spans="1:10" ht="48" customHeight="1">
-      <c r="A8" s="122" t="s">
+      <c r="A8" s="123" t="s">
         <v>452</v>
       </c>
       <c r="B8" s="63" t="s">
@@ -11259,7 +11277,7 @@
       <c r="J8" s="33"/>
     </row>
     <row r="9" spans="1:10" ht="15.6">
-      <c r="A9" s="122"/>
+      <c r="A9" s="123"/>
       <c r="B9" s="63" t="s">
         <v>455</v>
       </c>
@@ -11281,7 +11299,7 @@
       <c r="J9" s="33"/>
     </row>
     <row r="10" spans="1:10" ht="31.2">
-      <c r="A10" s="122"/>
+      <c r="A10" s="123"/>
       <c r="B10" s="63" t="s">
         <v>457</v>
       </c>
@@ -11301,7 +11319,7 @@
       <c r="J10" s="33"/>
     </row>
     <row r="11" spans="1:10" ht="62.4">
-      <c r="A11" s="122"/>
+      <c r="A11" s="123"/>
       <c r="B11" s="63" t="s">
         <v>459</v>
       </c>
@@ -11319,7 +11337,7 @@
       <c r="J11" s="33"/>
     </row>
     <row r="12" spans="1:10" ht="63.75" customHeight="1">
-      <c r="A12" s="122" t="s">
+      <c r="A12" s="123" t="s">
         <v>461</v>
       </c>
       <c r="B12" s="63" t="s">
@@ -11341,7 +11359,7 @@
       <c r="J12" s="33"/>
     </row>
     <row r="13" spans="1:10" ht="46.8">
-      <c r="A13" s="122"/>
+      <c r="A13" s="123"/>
       <c r="B13" s="63" t="s">
         <v>464</v>
       </c>
@@ -11361,7 +11379,7 @@
       <c r="J13" s="33"/>
     </row>
     <row r="14" spans="1:10" ht="46.8">
-      <c r="A14" s="122"/>
+      <c r="A14" s="123"/>
       <c r="B14" s="63" t="s">
         <v>466</v>
       </c>
@@ -11456,7 +11474,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="123" t="s">
         <v>468</v>
       </c>
       <c r="B2" s="63" t="s">
@@ -11478,7 +11496,7 @@
       <c r="J2" s="66"/>
     </row>
     <row r="3" spans="1:10" ht="46.8">
-      <c r="A3" s="122"/>
+      <c r="A3" s="123"/>
       <c r="B3" s="63" t="s">
         <v>471</v>
       </c>
@@ -11498,7 +11516,7 @@
       <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:10" ht="31.2">
-      <c r="A4" s="122"/>
+      <c r="A4" s="123"/>
       <c r="B4" s="63" t="s">
         <v>473</v>
       </c>
@@ -11518,7 +11536,7 @@
       <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="31.2">
-      <c r="A5" s="122"/>
+      <c r="A5" s="123"/>
       <c r="B5" s="63" t="s">
         <v>475</v>
       </c>
@@ -11538,7 +11556,7 @@
       <c r="J5" s="33"/>
     </row>
     <row r="6" spans="1:10" ht="31.2">
-      <c r="A6" s="122"/>
+      <c r="A6" s="123"/>
       <c r="B6" s="63" t="s">
         <v>477</v>
       </c>
@@ -11558,7 +11576,7 @@
       <c r="J6" s="33"/>
     </row>
     <row r="7" spans="1:10" ht="15.6">
-      <c r="A7" s="122"/>
+      <c r="A7" s="123"/>
       <c r="B7" s="63" t="s">
         <v>479</v>
       </c>
@@ -11578,7 +11596,7 @@
       <c r="J7" s="33"/>
     </row>
     <row r="8" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A8" s="122" t="s">
+      <c r="A8" s="123" t="s">
         <v>481</v>
       </c>
       <c r="B8" s="63" t="s">
@@ -11600,7 +11618,7 @@
       <c r="J8" s="33"/>
     </row>
     <row r="9" spans="1:10" ht="31.2">
-      <c r="A9" s="122"/>
+      <c r="A9" s="123"/>
       <c r="B9" s="63" t="s">
         <v>484</v>
       </c>
@@ -11620,7 +11638,7 @@
       <c r="J9" s="33"/>
     </row>
     <row r="10" spans="1:10" ht="31.2">
-      <c r="A10" s="122"/>
+      <c r="A10" s="123"/>
       <c r="B10" s="63" t="s">
         <v>486</v>
       </c>
@@ -11640,7 +11658,7 @@
       <c r="J10" s="33"/>
     </row>
     <row r="11" spans="1:10" ht="32.25" customHeight="1">
-      <c r="A11" s="122" t="s">
+      <c r="A11" s="123" t="s">
         <v>488</v>
       </c>
       <c r="B11" s="63" t="s">
@@ -11662,7 +11680,7 @@
       <c r="J11" s="33"/>
     </row>
     <row r="12" spans="1:10" ht="15.6">
-      <c r="A12" s="122"/>
+      <c r="A12" s="123"/>
       <c r="B12" s="63" t="s">
         <v>491</v>
       </c>
@@ -11682,7 +11700,7 @@
       <c r="J12" s="33"/>
     </row>
     <row r="13" spans="1:10" ht="46.8">
-      <c r="A13" s="122"/>
+      <c r="A13" s="123"/>
       <c r="B13" s="63" t="s">
         <v>493</v>
       </c>
@@ -11702,7 +11720,7 @@
       <c r="J13" s="33"/>
     </row>
     <row r="14" spans="1:10" ht="46.8">
-      <c r="A14" s="122"/>
+      <c r="A14" s="123"/>
       <c r="B14" s="63" t="s">
         <v>495</v>
       </c>
@@ -11722,7 +11740,7 @@
       <c r="J14" s="33"/>
     </row>
     <row r="15" spans="1:10" ht="31.2">
-      <c r="A15" s="122"/>
+      <c r="A15" s="123"/>
       <c r="B15" s="63" t="s">
         <v>497</v>
       </c>
@@ -11742,7 +11760,7 @@
       <c r="J15" s="33"/>
     </row>
     <row r="16" spans="1:10" ht="31.2">
-      <c r="A16" s="122"/>
+      <c r="A16" s="123"/>
       <c r="B16" s="63" t="s">
         <v>499</v>
       </c>
@@ -11762,7 +11780,7 @@
       <c r="J16" s="33"/>
     </row>
     <row r="17" spans="1:10" ht="46.8">
-      <c r="A17" s="122"/>
+      <c r="A17" s="123"/>
       <c r="B17" s="63" t="s">
         <v>501</v>
       </c>
@@ -11782,7 +11800,7 @@
       <c r="J17" s="33"/>
     </row>
     <row r="18" spans="1:10" ht="31.2">
-      <c r="A18" s="122"/>
+      <c r="A18" s="123"/>
       <c r="B18" s="63" t="s">
         <v>503</v>
       </c>

</xml_diff>